<commit_message>
Fixing file check tests
</commit_message>
<xml_diff>
--- a/tests/assets/expected_xpt/file1.xlsx
+++ b/tests/assets/expected_xpt/file1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/python/sas7bdat_converter/tests/assets/xpt_files/expected/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/python/sas7bdat_converter/tests/assets/expected_xpt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D402F93-549E-F740-BA90-BA5B6C17FA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6051EA0D-26B9-C746-B64B-ED42675993B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,16 @@
     <t>irow</t>
   </si>
   <si>
-    <t xml:space="preserve"> trow</t>
+    <t>trow</t>
   </si>
   <si>
-    <t xml:space="preserve"> Some text</t>
+    <t>frow</t>
   </si>
   <si>
-    <t xml:space="preserve"> Some more test</t>
+    <t>Some text</t>
   </si>
   <si>
-    <t xml:space="preserve"> frow</t>
+    <t>Some more test</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -910,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>17.23</v>

</xml_diff>